<commit_message>
correction of remarks from the reviewer and small visual changes
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evgeniy\PycharmProjects\intellegent_placer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096650F4-0F78-4165-BB00-A41339AC95A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917C9C28-7C41-4AD9-837E-74B5496CC332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{A3F4441A-8919-4884-AED3-9122D08F2EC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>Предмет уже не помещается в многоугольник</t>
+  </si>
+  <si>
+    <t>45.jpg</t>
+  </si>
+  <si>
+    <t>46.jpg</t>
+  </si>
+  <si>
+    <t>Зажигалка в нож</t>
+  </si>
+  <si>
+    <t>Зажигалка в транспортир</t>
   </si>
 </sst>
 </file>
@@ -581,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C896441E-5293-4366-8CA9-33976826F5F6}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,6 +1012,28 @@
         <v>60</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>